<commit_message>
Major system updates: authentication fixes, user management, database setup, and comprehensive documentation
</commit_message>
<xml_diff>
--- a/data/submissions.xlsx
+++ b/data/submissions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="193">
   <si>
     <t>FM-P-001</t>
   </si>
@@ -439,6 +439,12 @@
     <t>N/A (feature enabled)</t>
   </si>
   <si>
+    <t>2025-09-19T06:50:42.176Z</t>
+  </si>
+  <si>
+    <t>4324</t>
+  </si>
+  <si>
     <t>draft</t>
   </si>
   <si>
@@ -493,7 +499,13 @@
     <t>2025-09-17T17:23:12.382Z</t>
   </si>
   <si>
-    <t>2025-09-17T16:30:58.095Z</t>
+    <t>2025-09-19T09:35:04.197Z</t>
+  </si>
+  <si>
+    <t>fdsgsd</t>
+  </si>
+  <si>
+    <t>tr</t>
   </si>
   <si>
     <t>Baseline &amp; Endline</t>
@@ -535,7 +547,10 @@
     <t>This is a test case</t>
   </si>
   <si>
-    <t>2025-09-17T17:43:49.268Z</t>
+    <t>2025-09-18T13:34:37.900Z</t>
+  </si>
+  <si>
+    <t>lk</t>
   </si>
   <si>
     <t>2025-09-17T17:46:19.004Z</t>
@@ -7910,7 +7925,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -7951,9 +7966,12 @@
         <v>11</v>
       </c>
       <c r="N149" t="s">
+        <v>12</v>
+      </c>
+      <c r="O149" t="s">
         <v>142</v>
       </c>
-      <c r="O149" t="s">
+      <c r="P149" t="s">
         <v>143</v>
       </c>
     </row>
@@ -7998,10 +8016,10 @@
         <v>18</v>
       </c>
       <c r="N150" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O150" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
@@ -8045,10 +8063,10 @@
         <v>18</v>
       </c>
       <c r="N151" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O151" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.25">
@@ -8092,10 +8110,10 @@
         <v>18</v>
       </c>
       <c r="N152" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O152" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
@@ -8139,19 +8157,19 @@
         <v>18</v>
       </c>
       <c r="N153" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O153" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="P153" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="Q153" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="R153" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.25">
@@ -8195,10 +8213,10 @@
         <v>18</v>
       </c>
       <c r="N154" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O154" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.25">
@@ -8242,10 +8260,10 @@
         <v>18</v>
       </c>
       <c r="N155" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O155" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.25">
@@ -8289,10 +8307,10 @@
         <v>18</v>
       </c>
       <c r="N156" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O156" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.25">
@@ -8336,10 +8354,10 @@
         <v>18</v>
       </c>
       <c r="N157" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O157" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.25">
@@ -8383,10 +8401,10 @@
         <v>18</v>
       </c>
       <c r="N158" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O158" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.25">
@@ -8430,10 +8448,10 @@
         <v>18</v>
       </c>
       <c r="N159" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O159" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.25">
@@ -8477,10 +8495,10 @@
         <v>18</v>
       </c>
       <c r="N160" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O160" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.25">
@@ -8524,10 +8542,10 @@
         <v>18</v>
       </c>
       <c r="N161" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O161" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.25">
@@ -8571,10 +8589,10 @@
         <v>18</v>
       </c>
       <c r="N162" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O162" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
@@ -8618,10 +8636,10 @@
         <v>18</v>
       </c>
       <c r="N163" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O163" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.25">
@@ -8665,10 +8683,10 @@
         <v>18</v>
       </c>
       <c r="N164" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O164" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.25">
@@ -8712,10 +8730,10 @@
         <v>18</v>
       </c>
       <c r="N165" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O165" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.25">
@@ -8759,10 +8777,10 @@
         <v>18</v>
       </c>
       <c r="N166" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O166" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.25">
@@ -8806,10 +8824,10 @@
         <v>18</v>
       </c>
       <c r="N167" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O167" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
@@ -8853,10 +8871,10 @@
         <v>18</v>
       </c>
       <c r="N168" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O168" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.25">
@@ -8900,10 +8918,10 @@
         <v>18</v>
       </c>
       <c r="N169" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O169" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.25">
@@ -8947,10 +8965,10 @@
         <v>18</v>
       </c>
       <c r="N170" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O170" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
@@ -8994,10 +9012,10 @@
         <v>18</v>
       </c>
       <c r="N171" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O171" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.25">
@@ -9041,10 +9059,10 @@
         <v>18</v>
       </c>
       <c r="N172" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O172" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.25">
@@ -9088,10 +9106,10 @@
         <v>18</v>
       </c>
       <c r="N173" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O173" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.25">
@@ -9135,10 +9153,10 @@
         <v>18</v>
       </c>
       <c r="N174" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O174" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
@@ -9182,10 +9200,10 @@
         <v>18</v>
       </c>
       <c r="N175" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O175" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.25">
@@ -9229,10 +9247,10 @@
         <v>18</v>
       </c>
       <c r="N176" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O176" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
@@ -9276,10 +9294,10 @@
         <v>18</v>
       </c>
       <c r="N177" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O177" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.25">
@@ -9323,10 +9341,10 @@
         <v>18</v>
       </c>
       <c r="N178" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O178" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.25">
@@ -9370,10 +9388,10 @@
         <v>18</v>
       </c>
       <c r="N179" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O179" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
@@ -9417,10 +9435,10 @@
         <v>18</v>
       </c>
       <c r="N180" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O180" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.25">
@@ -9464,10 +9482,10 @@
         <v>18</v>
       </c>
       <c r="N181" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O181" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">
@@ -9511,10 +9529,10 @@
         <v>18</v>
       </c>
       <c r="N182" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O182" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.25">
@@ -9558,10 +9576,10 @@
         <v>18</v>
       </c>
       <c r="N183" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O183" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.25">
@@ -9605,10 +9623,10 @@
         <v>18</v>
       </c>
       <c r="N184" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O184" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.25">
@@ -9652,10 +9670,10 @@
         <v>18</v>
       </c>
       <c r="N185" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O185" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.25">
@@ -9681,7 +9699,7 @@
         <v>5</v>
       </c>
       <c r="H186" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I186" t="s">
         <v>137</v>
@@ -9690,19 +9708,19 @@
         <v>8</v>
       </c>
       <c r="K186" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L186" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="M186" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N186" t="s">
         <v>12</v>
       </c>
       <c r="O186" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
@@ -9728,28 +9746,28 @@
         <v>31</v>
       </c>
       <c r="H187" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I187" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J187" t="s">
         <v>18</v>
       </c>
       <c r="K187" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L187" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M187" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N187" t="s">
         <v>12</v>
       </c>
       <c r="O187" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.25">
@@ -9790,16 +9808,16 @@
         <v>20</v>
       </c>
       <c r="M188" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N188" t="s">
         <v>22</v>
       </c>
       <c r="O188" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -9822,28 +9840,34 @@
         <v>31</v>
       </c>
       <c r="H189" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I189" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J189" t="s">
         <v>18</v>
       </c>
       <c r="K189" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L189" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M189" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N189" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="O189" t="s">
-        <v>160</v>
+        <v>162</v>
+      </c>
+      <c r="Q189" t="s">
+        <v>163</v>
+      </c>
+      <c r="R189" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
@@ -9866,7 +9890,7 @@
         <v>4</v>
       </c>
       <c r="G190" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H190" t="s">
         <v>18</v>
@@ -9881,16 +9905,16 @@
         <v>136</v>
       </c>
       <c r="L190" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M190" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="N190" t="s">
         <v>12</v>
       </c>
       <c r="O190" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
@@ -9916,10 +9940,10 @@
         <v>106</v>
       </c>
       <c r="H191" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I191" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J191" t="s">
         <v>18</v>
@@ -9928,16 +9952,16 @@
         <v>9</v>
       </c>
       <c r="L191" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="M191" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="N191" t="s">
         <v>32</v>
       </c>
       <c r="O191" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.25">
@@ -9972,22 +9996,22 @@
         <v>18</v>
       </c>
       <c r="K192" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="L192" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="M192" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="N192" t="s">
         <v>32</v>
       </c>
       <c r="O192" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>0</v>
       </c>
@@ -10010,7 +10034,7 @@
         <v>5</v>
       </c>
       <c r="H193" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="I193" t="s">
         <v>137</v>
@@ -10019,19 +10043,22 @@
         <v>135</v>
       </c>
       <c r="K193" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L193" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M193" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="N193" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="O193" t="s">
-        <v>174</v>
+        <v>178</v>
+      </c>
+      <c r="Q193" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.25">
@@ -10057,7 +10084,7 @@
         <v>5</v>
       </c>
       <c r="H194" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="I194" t="s">
         <v>137</v>
@@ -10066,19 +10093,19 @@
         <v>135</v>
       </c>
       <c r="K194" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L194" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M194" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="N194" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O194" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.25">
@@ -10104,28 +10131,28 @@
         <v>106</v>
       </c>
       <c r="H195" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I195" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J195" t="s">
         <v>18</v>
       </c>
       <c r="K195" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="L195" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="M195" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="N195" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O195" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.25">
@@ -10151,28 +10178,28 @@
         <v>31</v>
       </c>
       <c r="H196" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I196" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J196" t="s">
         <v>18</v>
       </c>
       <c r="K196" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="L196" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="M196" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="N196" t="s">
         <v>32</v>
       </c>
       <c r="O196" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
@@ -10207,25 +10234,25 @@
         <v>8</v>
       </c>
       <c r="K197" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="L197" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="M197" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="N197" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O197" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="Q197" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="R197" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>